<commit_message>
Update TS for TC002 search func, update summary rerport
</commit_message>
<xml_diff>
--- a/Test Summary Report.xlsx
+++ b/Test Summary Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SENIUM WITH JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3E2BB4-6E25-4092-8370-B4DADBA89BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3C8609-539B-4510-8525-B9196C310657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{E28AEBC4-528C-4190-9FEA-BFE86C8B68D0}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Environment</t>
   </si>
@@ -180,16 +180,30 @@
   </si>
   <si>
     <t>Search Sneakers</t>
+  </si>
+  <si>
+    <t>HISTORY OF AMENDMENTS</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>New Update</t>
+  </si>
+  <si>
+    <t>- Judge passed/failed for search function manual test cases
+- Update Summary Report for search function lines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,8 +313,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +371,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -671,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -752,125 +780,173 @@
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2397,16 +2473,16 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B5:L15"/>
+  <dimension ref="B5:L49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U50" sqref="U50"/>
+      <selection activeCell="U61" sqref="U61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -2518,8 +2594,162 @@
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
     </row>
+    <row r="20" spans="2:12" ht="21" x14ac:dyDescent="0.4">
+      <c r="B20" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+    </row>
+    <row r="21" spans="2:12" ht="21" x14ac:dyDescent="0.4">
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="72"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="76"/>
+    </row>
+    <row r="23" spans="2:12" s="70" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="83">
+        <f ca="1">NOW()</f>
+        <v>44532.90596423611</v>
+      </c>
+      <c r="C23" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="85"/>
+    </row>
+    <row r="24" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="79"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="82"/>
+    </row>
+    <row r="25" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="79"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="81"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="80"/>
+      <c r="L25" s="82"/>
+    </row>
+    <row r="26" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="79"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="81"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="80"/>
+      <c r="L26" s="82"/>
+    </row>
+    <row r="27" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="79"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="81"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="80"/>
+      <c r="L27" s="82"/>
+    </row>
+    <row r="28" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="19">
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="K23:L23"/>
     <mergeCell ref="C15:L15"/>
     <mergeCell ref="C10:L10"/>
     <mergeCell ref="C11:L11"/>
@@ -2528,7 +2758,8 @@
     <mergeCell ref="C14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2540,7 +2771,7 @@
   <dimension ref="B2:N278"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R76" sqref="R76"/>
+      <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2554,21 +2785,21 @@
   <sheetData>
     <row r="2" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:14" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7"/>
@@ -2586,42 +2817,42 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="63"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="2:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="65"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="67"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2636,50 +2867,50 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="69"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="30">
         <f>SUM(D21:D30)</f>
         <v>3</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="40"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="39">
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="30">
         <f>SUM(E21:E30)</f>
-        <v>2</v>
-      </c>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
+        <v>3</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -2687,19 +2918,19 @@
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="37"/>
-      <c r="C12" s="41" t="s">
+      <c r="B12" s="46"/>
+      <c r="C12" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44">
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51">
         <f>SUM(F21:F30)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="45"/>
-      <c r="I12" s="46"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="53"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -2710,16 +2941,16 @@
       <c r="B13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="54">
         <f>SUM(G21:G30)</f>
-        <v>1</v>
-      </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="48"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -2730,15 +2961,15 @@
       <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="56">
         <v>0</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="50"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="57"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -2746,7 +2977,7 @@
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -2757,10 +2988,10 @@
         <v>17</v>
       </c>
       <c r="F15" s="15"/>
-      <c r="G15" s="53" t="s">
+      <c r="G15" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="54"/>
+      <c r="H15" s="61"/>
       <c r="I15" s="16"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -2769,19 +3000,19 @@
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="52"/>
-      <c r="C16" s="55" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58">
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="65">
         <f>D15+F15+I15</f>
         <v>0</v>
       </c>
-      <c r="H16" s="59"/>
-      <c r="I16" s="60"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="67"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -2804,63 +3035,63 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="30" t="s">
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="33" t="s">
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="41" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="31" t="s">
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="33" t="s">
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="36" t="s">
+      <c r="J19" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="36" t="s">
+      <c r="K19" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="33" t="s">
+      <c r="L19" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="M19" s="33" t="s">
+      <c r="M19" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="N19" s="34"/>
+      <c r="N19" s="42"/>
     </row>
     <row r="20" spans="2:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
       <c r="E20" s="20" t="s">
         <v>11</v>
       </c>
@@ -2873,12 +3104,12 @@
       <c r="H20" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="35"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
     </row>
     <row r="21" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="21" t="s">
@@ -2891,11 +3122,11 @@
         <v>3</v>
       </c>
       <c r="E21" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="22"/>
       <c r="I21" s="23">
@@ -3117,12 +3348,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="D18:D20"/>
@@ -3138,14 +3371,12 @@
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="N18:N20"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="B9:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update manual TCs for sort sneakers func and Test Summary Report
</commit_message>
<xml_diff>
--- a/Test Summary Report.xlsx
+++ b/Test Summary Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SENIUM WITH JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3C8609-539B-4510-8525-B9196C310657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2F2AC1-675E-44FE-8463-4472EC1E2006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{E28AEBC4-528C-4190-9FEA-BFE86C8B68D0}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Environment</t>
   </si>
@@ -193,6 +193,13 @@
   <si>
     <t>- Judge passed/failed for search function manual test cases
 - Update Summary Report for search function lines</t>
+  </si>
+  <si>
+    <t>Sort Sneakers</t>
+  </si>
+  <si>
+    <t>- Judge passed/failed for sort function manual test cases
+- Update Summary Report for sort function lines (4 cases being failed)</t>
   </si>
 </sst>
 </file>
@@ -201,7 +208,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -771,6 +778,54 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -780,12 +835,99 @@
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -812,141 +954,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2476,7 +2483,7 @@
   <dimension ref="B5:L49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U61" sqref="U61"/>
+      <selection activeCell="P80" sqref="P80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2498,226 +2505,231 @@
       <c r="B10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
     </row>
     <row r="11" spans="2:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
     </row>
     <row r="12" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
     </row>
     <row r="13" spans="2:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
     </row>
     <row r="14" spans="2:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="45">
         <v>44532</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
     </row>
     <row r="15" spans="2:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
     </row>
     <row r="20" spans="2:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="71"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
     </row>
     <row r="21" spans="2:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
     </row>
     <row r="22" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="74" t="s">
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="L22" s="76"/>
-    </row>
-    <row r="23" spans="2:12" s="70" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="83">
-        <f ca="1">NOW()</f>
-        <v>44532.90596423611</v>
-      </c>
-      <c r="C23" s="77" t="s">
+      <c r="L22" s="40"/>
+    </row>
+    <row r="23" spans="2:12" s="27" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="31">
+        <v>44532.01666666667</v>
+      </c>
+      <c r="C23" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="84" t="s">
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="85"/>
-    </row>
-    <row r="24" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="79"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="81"/>
-      <c r="I24" s="81"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="82"/>
-    </row>
-    <row r="25" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="79"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="81"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="82"/>
-    </row>
-    <row r="26" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="79"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="81"/>
-      <c r="I26" s="81"/>
-      <c r="J26" s="82"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="82"/>
-    </row>
-    <row r="27" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="79"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="81"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="82"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="82"/>
-    </row>
-    <row r="28" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="2:12" s="70" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="L23" s="42"/>
+    </row>
+    <row r="24" spans="2:12" s="27" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="31">
+        <v>44534.948611111111</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L24" s="42"/>
+    </row>
+    <row r="25" spans="2:12" s="27" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="30"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="34"/>
+    </row>
+    <row r="26" spans="2:12" s="27" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="30"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="34"/>
+    </row>
+    <row r="27" spans="2:12" s="27" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="30"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="34"/>
+    </row>
+    <row r="28" spans="2:12" s="27" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:12" s="27" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:12" s="27" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:12" s="27" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:12" s="27" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2737,6 +2749,18 @@
     <row r="49" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="C10:L10"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="C12:L12"/>
+    <mergeCell ref="C13:L13"/>
+    <mergeCell ref="C14:L14"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="K23:L23"/>
     <mergeCell ref="C25:J25"/>
     <mergeCell ref="C26:J26"/>
     <mergeCell ref="C27:J27"/>
@@ -2744,18 +2768,6 @@
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="K27:L27"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="C10:L10"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="C12:L12"/>
-    <mergeCell ref="C13:L13"/>
-    <mergeCell ref="C14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2771,7 +2783,7 @@
   <dimension ref="B2:N278"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S56" sqref="S56"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2785,21 +2797,21 @@
   <sheetData>
     <row r="2" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:14" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7"/>
@@ -2817,42 +2829,42 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="79"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="2:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="36"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="81"/>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="83"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2867,50 +2879,50 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="40"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="85"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="55">
         <f>SUM(D21:D30)</f>
-        <v>3</v>
-      </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
+        <v>7</v>
+      </c>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="30">
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="55">
         <f>SUM(E21:E30)</f>
         <v>3</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="31"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="56"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -2918,19 +2930,19 @@
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="46"/>
-      <c r="C12" s="48" t="s">
+      <c r="B12" s="53"/>
+      <c r="C12" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51">
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60">
         <f>SUM(F21:F30)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="52"/>
-      <c r="I12" s="53"/>
+        <v>4</v>
+      </c>
+      <c r="H12" s="61"/>
+      <c r="I12" s="62"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -2941,16 +2953,16 @@
       <c r="B13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="63">
         <f>SUM(G21:G30)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="55"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="64"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -2961,15 +2973,15 @@
       <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="65">
         <v>0</v>
       </c>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="57"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="66"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -2977,7 +2989,7 @@
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="67" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -2988,10 +3000,10 @@
         <v>17</v>
       </c>
       <c r="F15" s="15"/>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="61"/>
+      <c r="H15" s="70"/>
       <c r="I15" s="16"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -3000,19 +3012,19 @@
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="59"/>
-      <c r="C16" s="62" t="s">
+      <c r="B16" s="68"/>
+      <c r="C16" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65">
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="74">
         <f>D15+F15+I15</f>
         <v>0</v>
       </c>
-      <c r="H16" s="66"/>
-      <c r="I16" s="67"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="76"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -3035,63 +3047,63 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="68" t="s">
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="41" t="s">
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="44" t="s">
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="41" t="s">
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="69" t="s">
+      <c r="J19" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="69" t="s">
+      <c r="K19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="41" t="s">
+      <c r="L19" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="M19" s="41" t="s">
+      <c r="M19" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="N19" s="42"/>
+      <c r="N19" s="50"/>
     </row>
     <row r="20" spans="2:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="20" t="s">
         <v>11</v>
       </c>
@@ -3104,12 +3116,12 @@
       <c r="H20" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="43"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
     </row>
     <row r="21" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="21" t="s">
@@ -3124,11 +3136,15 @@
       <c r="E21" s="22">
         <v>3</v>
       </c>
-      <c r="F21" s="22"/>
+      <c r="F21" s="22">
+        <v>0</v>
+      </c>
       <c r="G21" s="22">
         <v>0</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="22">
+        <v>0</v>
+      </c>
       <c r="I21" s="23">
         <f>IFERROR(F21/D21,0)</f>
         <v>0</v>
@@ -3143,16 +3159,30 @@
       <c r="N21" s="25"/>
     </row>
     <row r="22" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="B22" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="22">
+        <v>4</v>
+      </c>
+      <c r="E22" s="22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="22">
+        <v>4</v>
+      </c>
+      <c r="G22" s="22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="22">
+        <v>0</v>
+      </c>
       <c r="I22" s="23">
         <f t="shared" ref="I22:I30" si="0">IFERROR(F22/D22,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="26"/>
       <c r="K22" s="26"/>
@@ -3348,14 +3378,12 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="N18:N20"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="B9:I9"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="D18:D20"/>
@@ -3371,12 +3399,14 @@
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="G16:I16"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>